<commit_message>
Add updated rubric tracker
</commit_message>
<xml_diff>
--- a/admin/ProjectRubric3of3.xlsx
+++ b/admin/ProjectRubric3of3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elari\Documents\Repos\CSCI_S71\Teamify\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6862BC8F-F2F9-456F-ACBA-F95AD4267567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7281F81-E535-4E43-989E-60D28B9304E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17055" yWindow="-15795" windowWidth="24075" windowHeight="15165" xr2:uid="{240F924D-48B8-43CB-A5F6-3B6DFA99720D}"/>
+    <workbookView xWindow="18855" yWindow="-16185" windowWidth="22590" windowHeight="15720" xr2:uid="{240F924D-48B8-43CB-A5F6-3B6DFA99720D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
   <si>
     <t>2.0 pts</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>Rubric Tracking for Assignment 3:  Final Sprint</t>
+  </si>
+  <si>
+    <t>Completed as Specified. README updated.</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -245,7 +251,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -580,10 +607,10 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -627,7 +654,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E4" s="2">
+        <v>44018</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -638,7 +671,13 @@
         <v>4</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E5" s="2">
+        <v>44018</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -649,7 +688,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E6" s="2">
+        <v>44018</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -660,7 +705,13 @@
         <v>0</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E7" s="2">
+        <v>44018</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -671,7 +722,13 @@
         <v>2</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E8" s="2">
+        <v>44018</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
@@ -682,7 +739,13 @@
         <v>10</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E9" s="2">
+        <v>44020</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -693,7 +756,13 @@
         <v>3</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E10" s="2">
+        <v>44020</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -704,7 +773,13 @@
         <v>3</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E11" s="2">
+        <v>44020</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -715,7 +790,13 @@
         <v>3</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E12" s="2">
+        <v>44020</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -726,7 +807,13 @@
         <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E13" s="2">
+        <v>44020</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -737,7 +824,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E14" s="2">
+        <v>44020</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -748,7 +841,13 @@
         <v>3</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>25</v>
+        <v>41</v>
+      </c>
+      <c r="E15" s="2">
+        <v>44020</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
@@ -906,7 +1005,18 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D1:D14 D16:D1048576">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"Deferred"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Pending"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"Complete"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Deferred"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Add presentation slides, add updated rubric
</commit_message>
<xml_diff>
--- a/admin/ProjectRubric3of3.xlsx
+++ b/admin/ProjectRubric3of3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elari\Documents\Repos\CSCI_S71\Teamify\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7281F81-E535-4E43-989E-60D28B9304E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A50F4EC-5903-4E98-B316-DBE9C1059D39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18855" yWindow="-16185" windowWidth="22590" windowHeight="15720" xr2:uid="{240F924D-48B8-43CB-A5F6-3B6DFA99720D}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{240F924D-48B8-43CB-A5F6-3B6DFA99720D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="42">
   <si>
     <t>2.0 pts</t>
   </si>
@@ -110,9 +110,6 @@
     <t>11.0 pts</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>There is evidence that you are building your product test-first. There is at least 1 BDD / A-TDD test in your suite, and it passes. (Fall semester: There are at least 3 BDD / A-TDD tests in your test suite (at least 1 new one this sprint), and it passes.) There are at least 30 unit tests in your test suite (at least 10 new unit tests this sprint), and they all pass.</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Completed as Specified.</t>
   </si>
 </sst>
 </file>
@@ -607,10 +607,10 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -626,7 +626,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -654,13 +654,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E4" s="2">
         <v>44018</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -671,13 +671,13 @@
         <v>4</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="2">
         <v>44018</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -688,13 +688,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2">
         <v>44018</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -705,13 +705,13 @@
         <v>0</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="2">
         <v>44018</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -722,13 +722,13 @@
         <v>2</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2">
         <v>44018</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="158.4" x14ac:dyDescent="0.55000000000000004">
@@ -739,13 +739,13 @@
         <v>10</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="2">
         <v>44020</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -756,13 +756,13 @@
         <v>3</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="2">
         <v>44020</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -773,13 +773,13 @@
         <v>3</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="2">
         <v>44020</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -790,13 +790,13 @@
         <v>3</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="2">
         <v>44020</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -807,13 +807,13 @@
         <v>2</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13" s="2">
         <v>44020</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -824,13 +824,13 @@
         <v>0</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="2">
         <v>44020</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -841,93 +841,135 @@
         <v>3</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="2">
         <v>44020</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="115.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E16" s="2">
+        <v>44020</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="144" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E17" s="2">
+        <v>44020</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="144" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E18" s="2">
+        <v>44020</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E19" s="2">
+        <v>44021</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E20" s="2">
+        <v>44021</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E21" s="2">
+        <v>44021</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E22" s="2">
+        <v>44021</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="7" t="s">
         <v>22</v>
       </c>
@@ -935,73 +977,115 @@
         <v>1</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E23" s="2">
+        <v>44020</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E24" s="2">
+        <v>44021</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E25" s="2">
+        <v>44021</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E26" s="2">
+        <v>44021</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E27" s="2">
+        <v>44021</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+      <c r="E28" s="2">
+        <v>44021</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="E29" s="2">
+        <v>44021</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>